<commit_message>
Added required fields and other fixes
-Unified WavelenghtRange
-Added LEDModule
-Changed cardinality for AnnotationRef
-Eliminated redundant Descriptions
-Added additional ChildrenElement category
-Clarified the difference between Ref and Sub-Element
</commit_message>
<xml_diff>
--- a/Tier System/v01-00/4DN-Metadata Tier System_2019-3-22_v01-00.xlsx
+++ b/Tier System/v01-00/4DN-Metadata Tier System_2019-3-22_v01-00.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Tier system_v03" sheetId="1" r:id="rId1"/>
-    <sheet name="Tier system_v03_SUBSET" sheetId="2" r:id="rId2"/>
+    <sheet name="Tier system_v01-00" sheetId="1" r:id="rId1"/>
+    <sheet name="Tier system_v01-00_SUMMARY" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,34 +19,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Caterina Strambio De Castillia</author>
-  </authors>
-  <commentList>
-    <comment ref="C7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Alternative designation:
-Development 
-Wizard
-Unicorn</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>-- required metadata --</t>
   </si>
@@ -249,12 +223,21 @@
   <si>
     <t>Detector calibration</t>
   </si>
+  <si>
+    <t>FISH, Immuno Fluorescence, Expression of FP</t>
+  </si>
+  <si>
+    <t>Pioneer</t>
+  </si>
+  <si>
+    <t>Development of novel unproved technology or of new gold-standard; full reproducibility ofmicroscopy set up and image acquisition settings</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -291,12 +274,6 @@
       <sz val="12"/>
       <color rgb="FF1B3641"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -607,10 +584,10 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -686,60 +663,66 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -750,12 +733,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1091,14 +1068,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1116,11 +1093,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
     </row>
     <row r="2" spans="1:12" ht="20" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1174,7 +1151,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>17</v>
@@ -1256,10 +1233,10 @@
       <c r="I5" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="46"/>
+      <c r="K5" s="48"/>
       <c r="L5" s="14"/>
     </row>
     <row r="6" spans="1:12" ht="90" customHeight="1">
@@ -1306,13 +1283,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>51</v>
@@ -1323,11 +1300,11 @@
       <c r="H7" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
       <c r="L7" s="14"/>
     </row>
     <row r="8" spans="1:12">
@@ -1346,7 +1323,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1362,7 +1338,7 @@
   </sheetPr>
   <dimension ref="A2:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -1383,25 +1359,25 @@
   <sheetData>
     <row r="2" spans="1:12" s="29" customFormat="1" ht="48" customHeight="1" thickBot="1">
       <c r="A2"/>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="49" t="s">
+      <c r="G2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="46" t="s">
         <v>58</v>
       </c>
       <c r="I2" s="28"/>

</xml_diff>